<commit_message>
Read data form excel - Raed
</commit_message>
<xml_diff>
--- a/Node.js/Projects/Read-Excel-File/assets/bgmi.xlsx
+++ b/Node.js/Projects/Read-Excel-File/assets/bgmi.xlsx
@@ -130,7 +130,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -162,16 +162,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -487,16 +484,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="32.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="32.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,8 +516,8 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -535,15 +532,15 @@
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>7077971352</v>
       </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1">
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -558,15 +555,15 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="1">
         <v>8480185421</v>
       </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1">
         <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -581,15 +578,15 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="1">
         <v>6372492300</v>
       </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1">
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -604,15 +601,15 @@
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>6371762801</v>
       </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1">
         <v>108</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -627,15 +624,15 @@
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>9777565564</v>
       </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1">
         <v>109</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -650,15 +647,15 @@
       <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>7008375219</v>
       </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3">
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1">
         <v>144</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -673,10 +670,10 @@
       <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>6372219368</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>